<commit_message>
new version for upper
</commit_message>
<xml_diff>
--- a/historical version.xlsx
+++ b/historical version.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\唐博\Desktop\CSharp-SerialPort-Helper-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\52775\Desktop\master_arbeit\EIS-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388BF901-F5EE-4151-AD14-D4F77E956A45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BE9B33-6B1F-4D52-AA09-5222563619F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4044" yWindow="2412" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="1635" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>version Nr.:</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -72,6 +72,29 @@
   <si>
     <t>Readme.txt</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v.2.0.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更新版本，频域和时域初步编写完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>实现具体实验参数传输</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>见Readme</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.与STM32数据传输还存在问题2.实验日期输入模式仍需修改</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>version2.0.1Readme.TXT</t>
   </si>
 </sst>
 </file>
@@ -218,7 +241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -243,9 +266,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -256,10 +276,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -540,19 +569,19 @@
   <dimension ref="B1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16:J16"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.88671875" customWidth="1"/>
-    <col min="3" max="3" width="27.21875" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" customWidth="1"/>
-    <col min="11" max="11" width="21.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.875" customWidth="1"/>
+    <col min="3" max="3" width="27.25" customWidth="1"/>
+    <col min="4" max="4" width="24.5" customWidth="1"/>
+    <col min="11" max="11" width="21.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -566,317 +595,329 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
-      <c r="K2" s="13"/>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K2" s="12"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7" t="s">
+      <c r="E3" s="14"/>
+      <c r="F3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7" t="s">
+      <c r="G3" s="14"/>
+      <c r="H3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
       <c r="K3" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="82.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="82.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7" t="s">
+      <c r="E4" s="14"/>
+      <c r="F4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7" t="s">
+      <c r="G4" s="14"/>
+      <c r="H4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="14" t="s">
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="8"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
       <c r="K6" s="8"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
       <c r="K7" s="8"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
       <c r="K8" s="8"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="4"/>
       <c r="C12" s="5"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
       <c r="K13" s="8"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
       <c r="K15" s="8"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
       <c r="K16" s="8"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
       <c r="K17" s="8"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
       <c r="K18" s="8"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
       <c r="K19" s="8"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
       <c r="K20" s="8"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
       <c r="K21" s="8"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
       <c r="K22" s="8"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
       <c r="K23" s="8"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" s="4"/>
       <c r="C24" s="5"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
       <c r="K24" s="8"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" s="4"/>
       <c r="C25" s="5"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
       <c r="K25" s="8"/>
     </row>
-    <row r="26" spans="2:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="9"/>
       <c r="C26" s="10"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="12"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="11"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
@@ -965,8 +1006,9 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="K4" r:id="rId1" xr:uid="{14BDEF56-04DA-45D2-8D4C-09506AFAC11C}"/>
+    <hyperlink ref="K5" r:id="rId2" xr:uid="{2A18AB35-EFA5-4400-826D-BF7008AA8C48}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>